<commit_message>
Mise à jour de la génération des rapport quantification invisible
Mise à jour de la génération des rapport quantification invisible
</commit_message>
<xml_diff>
--- a/apps/Exemple_rapport_thermique/Quantification_Statistique_thermique_exemple.xlsx
+++ b/apps/Exemple_rapport_thermique/Quantification_Statistique_thermique_exemple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAMER\Documents\Projects\vocasara4\Vocasar4\vocasara_webapp_update\Vocasara-full-app\Webapp - final version (correct) - Copie\Exemple_rapport_thermique\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAMER\Desktop\VocaSaraAppV2\apps\Exemple_rapport_thermique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3CD0EF-E194-48D8-9E74-16562D27575E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3E7E1B-2FD8-4DE8-8337-DABD665EB1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{D279A320-AABE-5B4F-9DCF-82F8663052E9}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11835" firstSheet="1" activeTab="1" xr2:uid="{D279A320-AABE-5B4F-9DCF-82F8663052E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" state="hidden" r:id="rId1"/>
@@ -64,10 +64,10 @@
     <t>Nom :</t>
   </si>
   <si>
+    <t xml:space="preserve">QUANTIFICATION STATISTIQUE DES DEFAUTS VISIBLES DE VISITES DES LIGNES HTA DANS LA ZONE (zone) PAR DRONE DU FEEDER (feeder) DE LA DATE DU (date)                           </t>
+  </si>
+  <si>
     <t>Defaut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUANTIFICATION STATISTIQUE DES DEFAUTS INSIBLES DE VISITES DES LIGNES HTA DANS LA ZONE (zone) PAR DRONE DU FEEDER (feeder) DE LA DATE DU (date)                           </t>
   </si>
   <si>
     <t>Température moyenne</t>
@@ -128,7 +128,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -780,7 +780,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -788,8 +788,8 @@
     <col min="1" max="1" width="20.375" customWidth="1"/>
     <col min="2" max="2" width="19.625" customWidth="1"/>
     <col min="3" max="3" width="60.75" customWidth="1"/>
-    <col min="4" max="4" width="42.125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="61.5" style="11" customWidth="1"/>
+    <col min="4" max="4" width="17" style="11" customWidth="1"/>
+    <col min="5" max="5" width="25.875" style="11" customWidth="1"/>
     <col min="6" max="6" width="31.125" customWidth="1"/>
     <col min="7" max="7" width="11.75" customWidth="1"/>
     <col min="8" max="8" width="30.875" customWidth="1"/>
@@ -800,7 +800,7 @@
       <c r="A1" s="19"/>
       <c r="B1" s="20"/>
       <c r="C1" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
@@ -907,7 +907,7 @@
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="31" t="s">

</xml_diff>